<commit_message>
add new docker image
</commit_message>
<xml_diff>
--- a/Template/data.xlsx
+++ b/Template/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\Perso\cyber-infra\docker-infra\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB34D8A3-1F72-4597-B509-DF2A4C3DC687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE50ADCD-F587-4D2F-A3F2-37002A23C3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3780" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="47">
   <si>
     <t>Total</t>
   </si>
@@ -147,9 +147,6 @@
     <t>NB étudiant</t>
   </si>
   <si>
-    <t>Alice</t>
-  </si>
-  <si>
     <t>Anatol</t>
   </si>
   <si>
@@ -159,16 +156,16 @@
     <t>Arange</t>
   </si>
   <si>
-    <t>Bob</t>
-  </si>
-  <si>
     <t>Barnon</t>
   </si>
   <si>
-    <t>Barille</t>
-  </si>
-  <si>
     <t>Bill</t>
+  </si>
+  <si>
+    <t>billiab</t>
+  </si>
+  <si>
+    <t>chali</t>
   </si>
 </sst>
 </file>
@@ -519,7 +516,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V28" sqref="V28"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,7 +534,7 @@
         <v>34</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -545,7 +542,7 @@
         <v>38</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -553,7 +550,7 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -604,16 +601,16 @@
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -621,67 +618,139 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
         <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
       <c r="D10" t="s">
         <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
       <c r="D11" t="s">
         <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
       <c r="D12" t="s">
         <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
       <c r="D13" t="s">
         <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
       <c r="D14" t="s">
         <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
       <c r="D15" t="s">
         <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>